<commit_message>
Adding test case 539 to regression
</commit_message>
<xml_diff>
--- a/test_files/Codelist_special_characters_for_codes.xlsx
+++ b/test_files/Codelist_special_characters_for_codes.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22123"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22206"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0F1898C9-6EE1-4B25-931B-B206660D398F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D2023AF-1DAD-46FF-AE4F-0850588341E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CodeSchemes" sheetId="1" r:id="rId1"/>
     <sheet name="Links_T100" sheetId="2" r:id="rId2"/>
     <sheet name="Codes_T100" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcCompleted="0" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="85">
   <si>
     <t>CODEVALUE</t>
   </si>
@@ -271,6 +271,15 @@
   </si>
   <si>
     <t>2018-02-06</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>piste</t>
+  </si>
+  <si>
+    <t>2018-02-07</t>
   </si>
 </sst>
 </file>
@@ -278,7 +287,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="1">
     <font>
@@ -311,7 +320,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -783,7 +792,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -899,10 +908,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1110,6 +1119,23 @@
         <v>44087</v>
       </c>
     </row>
+    <row r="7" spans="1:15">
+      <c r="A7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" t="s">
+        <v>83</v>
+      </c>
+      <c r="K7" t="s">
+        <v>84</v>
+      </c>
+      <c r="L7" s="1">
+        <v>44088</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>